<commit_message>
update to dashboard v2
</commit_message>
<xml_diff>
--- a/Data/Farmacia-entrenamiento.xlsx
+++ b/Data/Farmacia-entrenamiento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\Dashboard2\Dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AA1FE9-CAD7-461C-BA0F-9EFB0178F236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CCBF46-1063-41DC-BB65-A466786782AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4B218E8-29A0-4AC9-953F-8373C5594BCC}"/>
   </bookViews>
@@ -456,7 +456,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7E9E97-DA5C-4CAC-B229-E64E22364428}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -501,7 +503,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>0.4</v>

</xml_diff>